<commit_message>
devanagari and bengali are separated internally
</commit_message>
<xml_diff>
--- a/PUA_allocation_chart.xlsx
+++ b/PUA_allocation_chart.xlsx
@@ -14,17 +14,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1640751300" val="1040" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1640751300" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1640751300" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1640751300"/>
+      <pm:revision xmlns:pm="smNativeData" day="1641886364" val="1040" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1641886364" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1641886364" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1641886364"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
   <si>
     <t>PUA Allocation Chart U+Fxxxx</t>
   </si>
@@ -107,7 +107,16 @@
     <t>F00F</t>
   </si>
   <si>
+    <t>Unassigned</t>
+  </si>
+  <si>
+    <t>Devanagari Presentation Forms</t>
+  </si>
+  <si>
     <t>Small ASCII Characters for Super/Subscript Composition Used Internally</t>
+  </si>
+  <si>
+    <t>Todo: these codes may be moved outside of Unicode or use its own codespace</t>
   </si>
   <si>
     <t>F800</t>
@@ -322,7 +331,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1640751300" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -337,7 +346,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1640751300" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -353,7 +362,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1640751300" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="300" lang="default" weight="bold"/>
@@ -369,7 +378,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1640751300" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -385,7 +394,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1640751300" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -400,7 +409,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1640751300" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -411,14 +420,15 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <i/>
       <color rgb="FF000000"/>
-      <sz val="8"/>
+      <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1640751300" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="160" lang="default"/>
-            <pm:cs face="Basic Roman" sz="160" lang="default"/>
-            <pm:ea face="Basic Roman" sz="160" lang="default"/>
+          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
+            <pm:cs face="Basic Roman" sz="220" lang="default"/>
+            <pm:ea face="Basic Roman" sz="220" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -443,7 +453,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1640751300" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -454,7 +464,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1640751300" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -465,7 +475,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1640751300" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -476,7 +486,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1640751300" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -487,7 +497,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1640751300" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -501,18 +511,18 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1640751300" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFE6E6E6"/>
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1640751300" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -534,7 +544,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300"/>
+          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
         </ext>
       </extLst>
     </border>
@@ -553,7 +563,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300">
+          <pm:border xmlns:pm="smNativeData" id="1641886364">
             <pm:line position="bottom" type="1" style="0" width="50" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
         </ext>
@@ -574,7 +584,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300">
+          <pm:border xmlns:pm="smNativeData" id="1641886364">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -595,7 +605,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300">
+          <pm:border xmlns:pm="smNativeData" id="1641886364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -619,7 +629,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300"/>
+          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
         </ext>
       </extLst>
     </border>
@@ -638,7 +648,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300">
+          <pm:border xmlns:pm="smNativeData" id="1641886364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -661,7 +671,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300">
+          <pm:border xmlns:pm="smNativeData" id="1641886364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
           </pm:border>
@@ -683,7 +693,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300">
+          <pm:border xmlns:pm="smNativeData" id="1641886364">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -706,7 +716,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300">
+          <pm:border xmlns:pm="smNativeData" id="1641886364">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -727,7 +737,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300"/>
+          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
         </ext>
       </extLst>
     </border>
@@ -746,7 +756,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1640751300"/>
+          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
         </ext>
       </extLst>
     </border>
@@ -758,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
@@ -815,6 +825,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -826,10 +839,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1640751300" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1641886364" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1640751300" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1641886364" count="6">
         <pm:color name="Color 24" rgb="44546A"/>
         <pm:color name="Color 25" rgb="FFFFCC"/>
         <pm:color name="Color 26" rgb="A5A5A5"/>
@@ -1098,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T70"/>
+  <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -1526,632 +1539,1635 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:18">
       <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="2:2">
+      <c r="C20" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+    </row>
+    <row r="21" spans="2:18">
       <c r="B21" s="7" t="str">
         <f>"F01"&amp;RIGHT(B5,1)</f>
         <v>F010</v>
       </c>
-    </row>
-    <row r="22" spans="2:2">
+      <c r="C21" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+    </row>
+    <row r="22" spans="2:18">
       <c r="B22" s="7" t="str">
         <f>"F01"&amp;RIGHT(B6,1)</f>
         <v>F011</v>
       </c>
-    </row>
-    <row r="23" spans="2:2">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+    </row>
+    <row r="23" spans="2:18">
       <c r="B23" s="7" t="str">
         <f>"F01"&amp;RIGHT(B7,1)</f>
         <v>F012</v>
       </c>
-    </row>
-    <row r="24" spans="2:2">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+    </row>
+    <row r="24" spans="2:18">
       <c r="B24" s="7" t="str">
         <f>"F01"&amp;RIGHT(B8,1)</f>
         <v>F013</v>
       </c>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+    </row>
+    <row r="25" spans="2:18">
       <c r="B25" s="7" t="str">
         <f>"F01"&amp;RIGHT(B9,1)</f>
         <v>F014</v>
       </c>
-    </row>
-    <row r="26" spans="2:2">
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+    </row>
+    <row r="26" spans="2:18">
       <c r="B26" s="7" t="str">
         <f>"F01"&amp;RIGHT(B10,1)</f>
         <v>F015</v>
       </c>
-    </row>
-    <row r="27" spans="2:2">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+    </row>
+    <row r="27" spans="2:18">
       <c r="B27" s="7" t="str">
         <f>"F01"&amp;RIGHT(B11,1)</f>
         <v>F016</v>
       </c>
-    </row>
-    <row r="28" spans="2:2">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+    </row>
+    <row r="28" spans="2:18">
       <c r="B28" s="7" t="str">
         <f>"F01"&amp;RIGHT(B12,1)</f>
         <v>F017</v>
       </c>
-    </row>
-    <row r="29" spans="2:2">
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+    </row>
+    <row r="29" spans="2:18">
       <c r="B29" s="7" t="str">
         <f>"F01"&amp;RIGHT(B13,1)</f>
         <v>F018</v>
       </c>
-    </row>
-    <row r="30" spans="2:2">
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+    </row>
+    <row r="30" spans="2:18">
       <c r="B30" s="7" t="str">
         <f>"F01"&amp;RIGHT(B14,1)</f>
         <v>F019</v>
       </c>
-    </row>
-    <row r="31" spans="2:2">
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+    </row>
+    <row r="31" spans="2:18">
       <c r="B31" s="7" t="str">
         <f>"F01"&amp;RIGHT(B15,1)</f>
         <v>F01A</v>
       </c>
-    </row>
-    <row r="32" spans="2:2">
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+    </row>
+    <row r="32" spans="2:18">
       <c r="B32" s="7" t="str">
         <f>"F01"&amp;RIGHT(B16,1)</f>
         <v>F01B</v>
       </c>
-    </row>
-    <row r="33" spans="2:2">
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+    </row>
+    <row r="33" spans="2:18">
       <c r="B33" s="7" t="str">
         <f>"F01"&amp;RIGHT(B17,1)</f>
         <v>F01C</v>
       </c>
-    </row>
-    <row r="34" spans="2:2">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+    </row>
+    <row r="34" spans="2:18">
       <c r="B34" s="7" t="str">
         <f>"F01"&amp;RIGHT(B18,1)</f>
         <v>F01D</v>
       </c>
-    </row>
-    <row r="35" spans="2:2">
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+    </row>
+    <row r="35" spans="2:18">
       <c r="B35" s="7" t="str">
         <f>"F01"&amp;RIGHT(B19,1)</f>
         <v>F01E</v>
       </c>
-    </row>
-    <row r="36" spans="2:2">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+    </row>
+    <row r="36" spans="2:18">
       <c r="B36" s="7" t="str">
         <f>"F01"&amp;RIGHT(B20,1)</f>
         <v>F01F</v>
       </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+    </row>
+    <row r="37" spans="2:18">
+      <c r="B37" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B21,1)</f>
+        <v>F020</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
     </row>
     <row r="38" spans="2:18">
-      <c r="B38" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
+      <c r="B38" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B22,1)</f>
+        <v>F021</v>
+      </c>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
     </row>
     <row r="39" spans="2:18">
-      <c r="B39" s="8"/>
-      <c r="C39" s="5" t="n">
+      <c r="B39" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B23,1)</f>
+        <v>F022</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+    </row>
+    <row r="40" spans="2:18">
+      <c r="B40" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B24,1)</f>
+        <v>F023</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+    </row>
+    <row r="41" spans="2:18">
+      <c r="B41" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B25,1)</f>
+        <v>F024</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+    </row>
+    <row r="42" spans="2:18">
+      <c r="B42" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B26,1)</f>
+        <v>F025</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+    </row>
+    <row r="43" spans="2:18">
+      <c r="B43" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B27,1)</f>
+        <v>F026</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+    </row>
+    <row r="44" spans="2:18">
+      <c r="B44" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B28,1)</f>
+        <v>F027</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+    </row>
+    <row r="45" spans="2:18">
+      <c r="B45" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B29,1)</f>
+        <v>F028</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+    </row>
+    <row r="46" spans="2:18">
+      <c r="B46" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B30,1)</f>
+        <v>F029</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+    </row>
+    <row r="47" spans="2:18">
+      <c r="B47" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B31,1)</f>
+        <v>F02A</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+    </row>
+    <row r="48" spans="2:18">
+      <c r="B48" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B32,1)</f>
+        <v>F02B</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+    </row>
+    <row r="49" spans="2:18">
+      <c r="B49" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B33,1)</f>
+        <v>F02C</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+    </row>
+    <row r="50" spans="2:18">
+      <c r="B50" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B34,1)</f>
+        <v>F02D</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
+    </row>
+    <row r="51" spans="2:18">
+      <c r="B51" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B35,1)</f>
+        <v>F02E</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
+    </row>
+    <row r="52" spans="2:18">
+      <c r="B52" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B36,1)</f>
+        <v>F02F</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+    </row>
+    <row r="53" spans="2:18">
+      <c r="B53" s="7" t="str">
+        <f>"F02"&amp;RIGHT(B37,1)</f>
+        <v>F020</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+    </row>
+    <row r="54" spans="2:18">
+      <c r="B54" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B38,1)</f>
+        <v>F031</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+    </row>
+    <row r="55" spans="2:18">
+      <c r="B55" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B39,1)</f>
+        <v>F032</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+    </row>
+    <row r="56" spans="2:18">
+      <c r="B56" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B40,1)</f>
+        <v>F033</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15"/>
+      <c r="O56" s="15"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="15"/>
+      <c r="R56" s="15"/>
+    </row>
+    <row r="57" spans="2:18">
+      <c r="B57" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B41,1)</f>
+        <v>F034</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
+      <c r="Q57" s="15"/>
+      <c r="R57" s="15"/>
+    </row>
+    <row r="58" spans="2:18">
+      <c r="B58" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B42,1)</f>
+        <v>F035</v>
+      </c>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
+      <c r="Q58" s="15"/>
+      <c r="R58" s="15"/>
+    </row>
+    <row r="59" spans="2:18">
+      <c r="B59" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B43,1)</f>
+        <v>F036</v>
+      </c>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="15"/>
+      <c r="R59" s="15"/>
+    </row>
+    <row r="60" spans="2:18">
+      <c r="B60" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B44,1)</f>
+        <v>F037</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
+      <c r="R60" s="15"/>
+    </row>
+    <row r="61" spans="2:18">
+      <c r="B61" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B45,1)</f>
+        <v>F038</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+    </row>
+    <row r="62" spans="2:18">
+      <c r="B62" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B46,1)</f>
+        <v>F039</v>
+      </c>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
+    </row>
+    <row r="63" spans="2:18">
+      <c r="B63" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B47,1)</f>
+        <v>F03A</v>
+      </c>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+      <c r="R63" s="15"/>
+    </row>
+    <row r="64" spans="2:18">
+      <c r="B64" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B48,1)</f>
+        <v>F03B</v>
+      </c>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
+    </row>
+    <row r="65" spans="2:18">
+      <c r="B65" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B49,1)</f>
+        <v>F03C</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
+    </row>
+    <row r="66" spans="2:18">
+      <c r="B66" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B50,1)</f>
+        <v>F03D</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="15"/>
+    </row>
+    <row r="67" spans="2:18">
+      <c r="B67" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B51,1)</f>
+        <v>F03E</v>
+      </c>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="15"/>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
+    </row>
+    <row r="68" spans="2:18">
+      <c r="B68" s="7" t="str">
+        <f>"F03"&amp;RIGHT(B52,1)</f>
+        <v>F03F</v>
+      </c>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
+    </row>
+    <row r="69" spans="3:18">
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+    </row>
+    <row r="71" spans="2:19">
+      <c r="B71" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+      <c r="J71" s="17"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
+      <c r="Q71" s="17"/>
+      <c r="R71" s="17"/>
+      <c r="S71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18">
+      <c r="B72" s="8"/>
+      <c r="C72" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D39" s="5" t="n">
+      <c r="D72" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E39" s="5" t="n">
+      <c r="E72" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F39" s="5" t="n">
+      <c r="F72" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G39" s="5" t="n">
+      <c r="G72" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H39" s="5" t="n">
+      <c r="H72" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I39" s="5" t="n">
+      <c r="I72" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J39" s="5" t="n">
+      <c r="J72" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K39" s="5" t="n">
+      <c r="K72" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L39" s="5" t="n">
+      <c r="L72" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="M72" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N39" s="5" t="s">
+      <c r="N72" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O39" s="5" t="s">
+      <c r="O72" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P39" s="5" t="s">
+      <c r="P72" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q39" s="5" t="s">
+      <c r="Q72" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R39" s="5" t="s">
+      <c r="R72" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="2:19">
-      <c r="B40" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S40" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="7" t="s">
+    <row r="73" spans="2:19">
+      <c r="B73" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="7" t="s">
+      <c r="S73" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="9" t="s">
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="7" t="s">
+      <c r="C74" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="9" t="s">
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="7" t="s">
+      <c r="C75" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="9" t="s">
+    </row>
+    <row r="76" spans="2:3">
+      <c r="B76" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="7" t="s">
+      <c r="C76" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="9" t="s">
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="2:18">
-      <c r="B47" s="17" t="s">
+      <c r="C77" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
-      <c r="Q47" s="17"/>
-      <c r="R47" s="17"/>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48" s="7" t="s">
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C78" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="7" t="s">
+    <row r="80" spans="2:18">
+      <c r="B80" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+      <c r="J80" s="17"/>
+      <c r="K80" s="17"/>
+      <c r="L80" s="17"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="17"/>
+      <c r="R80" s="17"/>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="B50" s="7" t="s">
+      <c r="C81" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="9" t="s">
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="B51" s="7" t="s">
+      <c r="C82" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="9" t="s">
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="2:3">
-      <c r="B52" s="7" t="s">
+      <c r="C83" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="9" t="s">
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" s="7" t="s">
+      <c r="C84" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="9" t="s">
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="2:18">
-      <c r="B55" s="11" t="s">
+      <c r="C85" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="13"/>
-    </row>
-    <row r="56" spans="2:18">
-      <c r="B56" s="8"/>
-      <c r="C56" s="5" t="n">
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18">
+      <c r="B88" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
+      <c r="L88" s="12"/>
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+      <c r="O88" s="12"/>
+      <c r="P88" s="12"/>
+      <c r="Q88" s="12"/>
+      <c r="R88" s="13"/>
+    </row>
+    <row r="89" spans="2:18">
+      <c r="B89" s="8"/>
+      <c r="C89" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D56" s="5" t="n">
+      <c r="D89" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E56" s="5" t="n">
+      <c r="E89" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F56" s="5" t="n">
+      <c r="F89" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G56" s="5" t="n">
+      <c r="G89" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H56" s="5" t="n">
+      <c r="H89" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I56" s="5" t="n">
+      <c r="I89" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J56" s="5" t="n">
+      <c r="J89" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K56" s="5" t="n">
+      <c r="K89" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L56" s="5" t="n">
+      <c r="L89" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M56" s="5" t="s">
+      <c r="M89" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N56" s="5" t="s">
+      <c r="N89" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O56" s="5" t="s">
+      <c r="O89" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P56" s="5" t="s">
+      <c r="P89" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q56" s="5" t="s">
+      <c r="Q89" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R56" s="5" t="s">
+      <c r="R89" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="2:20">
-      <c r="B57" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="S57" t="s">
+    <row r="90" spans="2:20">
+      <c r="B90" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="T57" t="s">
+      <c r="C90" s="9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="2:19">
-      <c r="B58" s="7" t="s">
+      <c r="D90" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="S90" t="s">
         <v>61</v>
       </c>
-      <c r="S58" t="s">
+      <c r="T90" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="2:18">
-      <c r="B60" s="11" t="s">
+    <row r="91" spans="2:19">
+      <c r="B91" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="K60" s="12"/>
-      <c r="L60" s="12"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12"/>
-      <c r="P60" s="12"/>
-      <c r="Q60" s="12"/>
-      <c r="R60" s="13"/>
-    </row>
-    <row r="61" spans="2:18">
-      <c r="B61" s="8"/>
-      <c r="C61" s="5" t="n">
+      <c r="C91" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="S91" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="2:18">
+      <c r="B93" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
+      <c r="L93" s="12"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="12"/>
+      <c r="P93" s="12"/>
+      <c r="Q93" s="12"/>
+      <c r="R93" s="13"/>
+    </row>
+    <row r="94" spans="2:18">
+      <c r="B94" s="8"/>
+      <c r="C94" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D61" s="5" t="n">
+      <c r="D94" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E61" s="5" t="n">
+      <c r="E94" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F61" s="5" t="n">
+      <c r="F94" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G61" s="5" t="n">
+      <c r="G94" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H61" s="5" t="n">
+      <c r="H94" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I61" s="5" t="n">
+      <c r="I94" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J61" s="5" t="n">
+      <c r="J94" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K61" s="5" t="n">
+      <c r="K94" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L61" s="5" t="n">
+      <c r="L94" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M61" s="5" t="s">
+      <c r="M94" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N61" s="5" t="s">
+      <c r="N94" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O61" s="5" t="s">
+      <c r="O94" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P61" s="5" t="s">
+      <c r="P94" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q61" s="5" t="s">
+      <c r="Q94" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R61" s="5" t="s">
+      <c r="R94" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="2:19">
-      <c r="B62" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E62" s="9" t="s">
+    <row r="95" spans="2:19">
+      <c r="B95" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="C95" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="S62" t="s">
+      <c r="D95" s="9" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="63" spans="2:19">
-      <c r="B63" s="7" t="s">
+      <c r="E95" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="R63" s="9" t="s">
+      <c r="F95" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="S63" t="s">
+      <c r="S95" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="2:18">
-      <c r="B65" s="11" t="s">
+    <row r="96" spans="2:19">
+      <c r="B96" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
-      <c r="M65" s="12"/>
-      <c r="N65" s="12"/>
-      <c r="O65" s="12"/>
-      <c r="P65" s="12"/>
-      <c r="Q65" s="12"/>
-      <c r="R65" s="13"/>
-    </row>
-    <row r="66" spans="2:18">
-      <c r="B66" s="8"/>
-      <c r="C66" s="5" t="n">
+      <c r="R96" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="S96" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18">
+      <c r="B98" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+      <c r="O98" s="12"/>
+      <c r="P98" s="12"/>
+      <c r="Q98" s="12"/>
+      <c r="R98" s="13"/>
+    </row>
+    <row r="99" spans="2:18">
+      <c r="B99" s="8"/>
+      <c r="C99" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D66" s="5" t="n">
+      <c r="D99" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E66" s="5" t="n">
+      <c r="E99" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F66" s="5" t="n">
+      <c r="F99" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G66" s="5" t="n">
+      <c r="G99" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H66" s="5" t="n">
+      <c r="H99" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I66" s="5" t="n">
+      <c r="I99" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J66" s="5" t="n">
+      <c r="J99" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K66" s="5" t="n">
+      <c r="K99" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L66" s="5" t="n">
+      <c r="L99" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M66" s="5" t="s">
+      <c r="M99" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N66" s="5" t="s">
+      <c r="N99" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O66" s="5" t="s">
+      <c r="O99" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P66" s="5" t="s">
+      <c r="P99" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q66" s="5" t="s">
+      <c r="Q99" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R66" s="5" t="s">
+      <c r="R99" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:5">
-      <c r="B67" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E67" s="9" t="s">
+    <row r="100" spans="2:5">
+      <c r="B100" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="7" t="s">
+      <c r="C100" s="9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="69" spans="2:2">
-      <c r="B69" s="7" t="s">
+      <c r="D100" s="9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="70" spans="2:2">
-      <c r="B70" s="7" t="s">
+      <c r="E100" s="9" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="B3:R3"/>
     <mergeCell ref="C5:R10"/>
     <mergeCell ref="C11:R16"/>
     <mergeCell ref="C17:R19"/>
-    <mergeCell ref="B38:R38"/>
-    <mergeCell ref="C40:R40"/>
-    <mergeCell ref="C41:R41"/>
-    <mergeCell ref="C42:R42"/>
-    <mergeCell ref="C43:R43"/>
-    <mergeCell ref="C44:R44"/>
-    <mergeCell ref="C45:R45"/>
-    <mergeCell ref="B47:R47"/>
-    <mergeCell ref="C48:R48"/>
-    <mergeCell ref="C49:R49"/>
-    <mergeCell ref="C50:R50"/>
-    <mergeCell ref="C51:R51"/>
-    <mergeCell ref="C52:R52"/>
-    <mergeCell ref="C53:R53"/>
-    <mergeCell ref="B55:R55"/>
-    <mergeCell ref="B60:R60"/>
-    <mergeCell ref="B65:R65"/>
+    <mergeCell ref="C20:R20"/>
+    <mergeCell ref="C21:R36"/>
+    <mergeCell ref="B71:R71"/>
+    <mergeCell ref="C73:R73"/>
+    <mergeCell ref="C74:R74"/>
+    <mergeCell ref="C75:R75"/>
+    <mergeCell ref="C76:R76"/>
+    <mergeCell ref="C77:R77"/>
+    <mergeCell ref="C78:R78"/>
+    <mergeCell ref="B80:R80"/>
+    <mergeCell ref="C81:R81"/>
+    <mergeCell ref="C82:R82"/>
+    <mergeCell ref="C83:R83"/>
+    <mergeCell ref="C84:R84"/>
+    <mergeCell ref="C85:R85"/>
+    <mergeCell ref="C86:R86"/>
+    <mergeCell ref="B88:R88"/>
+    <mergeCell ref="B93:R93"/>
+    <mergeCell ref="B98:R98"/>
   </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1640751300" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1641886364" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2160,14 +3176,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1640751300" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1640751300" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1640751300" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641886364" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2193,7 +3209,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="16" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -2288,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -2641,10 +3657,10 @@
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -2664,7 +3680,7 @@
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -2685,7 +3701,7 @@
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -2706,7 +3722,7 @@
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="21" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -2727,7 +3743,7 @@
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -2748,7 +3764,7 @@
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -2769,7 +3785,7 @@
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -2941,7 +3957,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1640751300" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1641886364" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2950,14 +3966,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1640751300" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1640751300" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1640751300" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641886364" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
devanagari: fixed the RAsup positioning
</commit_message>
<xml_diff>
--- a/PUA_allocation_chart.xlsx
+++ b/PUA_allocation_chart.xlsx
@@ -14,17 +14,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1641886364" val="1040" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1641886364" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1641886364" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1641886364"/>
+      <pm:revision xmlns:pm="smNativeData" day="1643161361" val="1040" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1643161361" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1643161361" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1643161361"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
   <si>
     <t>PUA Allocation Chart U+Fxxxx</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>Superscript Falsum Trademark</t>
+  </si>
+  <si>
+    <t>FFE2</t>
+  </si>
+  <si>
+    <t>IPA Intonation Graph Fragments</t>
+  </si>
+  <si>
+    <t>FFE3</t>
   </si>
   <si>
     <t>Rich Text Modifiers</t>
@@ -331,7 +340,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -346,7 +355,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -362,7 +371,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="300" lang="default" weight="bold"/>
@@ -378,7 +387,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -394,7 +403,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -409,7 +418,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -425,7 +434,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1641886364" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -453,7 +462,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -464,7 +473,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -475,7 +484,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -486,7 +495,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -497,7 +506,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -507,22 +516,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFE6E6E6"/>
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6E6"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1641886364" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -544,7 +553,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
+          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
         </ext>
       </extLst>
     </border>
@@ -563,7 +572,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364">
+          <pm:border xmlns:pm="smNativeData" id="1643161361">
             <pm:line position="bottom" type="1" style="0" width="50" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
         </ext>
@@ -584,7 +593,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364">
+          <pm:border xmlns:pm="smNativeData" id="1643161361">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -605,7 +614,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364">
+          <pm:border xmlns:pm="smNativeData" id="1643161361">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -629,7 +638,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
+          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
         </ext>
       </extLst>
     </border>
@@ -648,7 +657,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364">
+          <pm:border xmlns:pm="smNativeData" id="1643161361">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -671,7 +680,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364">
+          <pm:border xmlns:pm="smNativeData" id="1643161361">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
           </pm:border>
@@ -693,7 +702,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364">
+          <pm:border xmlns:pm="smNativeData" id="1643161361">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -716,7 +725,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364">
+          <pm:border xmlns:pm="smNativeData" id="1643161361">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -737,7 +746,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
+          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
         </ext>
       </extLst>
     </border>
@@ -756,7 +765,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1641886364"/>
+          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
         </ext>
       </extLst>
     </border>
@@ -825,7 +834,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -839,10 +848,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1641886364" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1643161361" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1641886364" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1643161361" count="6">
         <pm:color name="Color 24" rgb="44546A"/>
         <pm:color name="Color 25" rgb="FFFFCC"/>
         <pm:color name="Color 26" rgb="A5A5A5"/>
@@ -1111,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T103"/>
+  <dimension ref="A1:T105"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S72" sqref="S72"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -2933,208 +2942,252 @@
         <v>65</v>
       </c>
     </row>
+    <row r="92" spans="2:18">
+      <c r="B92" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
+      <c r="N92" s="15"/>
+      <c r="O92" s="15"/>
+      <c r="P92" s="15"/>
+      <c r="Q92" s="15"/>
+      <c r="R92" s="15"/>
+    </row>
     <row r="93" spans="2:18">
-      <c r="B93" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="12"/>
-      <c r="I93" s="12"/>
-      <c r="J93" s="12"/>
-      <c r="K93" s="12"/>
-      <c r="L93" s="12"/>
-      <c r="M93" s="12"/>
-      <c r="N93" s="12"/>
-      <c r="O93" s="12"/>
-      <c r="P93" s="12"/>
-      <c r="Q93" s="12"/>
-      <c r="R93" s="13"/>
-    </row>
-    <row r="94" spans="2:18">
-      <c r="B94" s="8"/>
-      <c r="C94" s="5" t="n">
+      <c r="B93" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" s="15"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="15"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
+      <c r="N93" s="15"/>
+      <c r="O93" s="15"/>
+      <c r="P93" s="15"/>
+      <c r="Q93" s="15"/>
+      <c r="R93" s="15"/>
+    </row>
+    <row r="95" spans="2:18">
+      <c r="B95" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
+      <c r="M95" s="12"/>
+      <c r="N95" s="12"/>
+      <c r="O95" s="12"/>
+      <c r="P95" s="12"/>
+      <c r="Q95" s="12"/>
+      <c r="R95" s="13"/>
+    </row>
+    <row r="96" spans="2:18">
+      <c r="B96" s="8"/>
+      <c r="C96" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D94" s="5" t="n">
+      <c r="D96" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E94" s="5" t="n">
+      <c r="E96" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F94" s="5" t="n">
+      <c r="F96" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G94" s="5" t="n">
+      <c r="G96" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H94" s="5" t="n">
+      <c r="H96" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I94" s="5" t="n">
+      <c r="I96" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J94" s="5" t="n">
+      <c r="J96" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K94" s="5" t="n">
+      <c r="K96" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L94" s="5" t="n">
+      <c r="L96" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M94" s="5" t="s">
+      <c r="M96" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N94" s="5" t="s">
+      <c r="N96" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O94" s="5" t="s">
+      <c r="O96" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P94" s="5" t="s">
+      <c r="P96" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q94" s="5" t="s">
+      <c r="Q96" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R94" s="5" t="s">
+      <c r="R96" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="2:19">
-      <c r="B95" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E95" s="9" t="s">
+    <row r="97" spans="2:19">
+      <c r="B97" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F95" s="9" t="s">
+      <c r="C97" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="S95" t="s">
+      <c r="D97" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="96" spans="2:19">
-      <c r="B96" s="7" t="s">
+      <c r="E97" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="R96" s="9" t="s">
+      <c r="F97" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="S96" t="s">
+      <c r="S97" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="2:18">
-      <c r="B98" s="11" t="s">
+    <row r="98" spans="2:19">
+      <c r="B98" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="12"/>
-      <c r="I98" s="12"/>
-      <c r="J98" s="12"/>
-      <c r="K98" s="12"/>
-      <c r="L98" s="12"/>
-      <c r="M98" s="12"/>
-      <c r="N98" s="12"/>
-      <c r="O98" s="12"/>
-      <c r="P98" s="12"/>
-      <c r="Q98" s="12"/>
-      <c r="R98" s="13"/>
-    </row>
-    <row r="99" spans="2:18">
-      <c r="B99" s="8"/>
-      <c r="C99" s="5" t="n">
+      <c r="R98" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="S98" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18">
+      <c r="B100" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12"/>
+      <c r="K100" s="12"/>
+      <c r="L100" s="12"/>
+      <c r="M100" s="12"/>
+      <c r="N100" s="12"/>
+      <c r="O100" s="12"/>
+      <c r="P100" s="12"/>
+      <c r="Q100" s="12"/>
+      <c r="R100" s="13"/>
+    </row>
+    <row r="101" spans="2:18">
+      <c r="B101" s="8"/>
+      <c r="C101" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D99" s="5" t="n">
+      <c r="D101" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E99" s="5" t="n">
+      <c r="E101" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F99" s="5" t="n">
+      <c r="F101" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G99" s="5" t="n">
+      <c r="G101" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H99" s="5" t="n">
+      <c r="H101" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I99" s="5" t="n">
+      <c r="I101" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J99" s="5" t="n">
+      <c r="J101" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K99" s="5" t="n">
+      <c r="K101" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L99" s="5" t="n">
+      <c r="L101" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M99" s="5" t="s">
+      <c r="M101" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N99" s="5" t="s">
+      <c r="N101" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O99" s="5" t="s">
+      <c r="O101" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P99" s="5" t="s">
+      <c r="P101" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q99" s="5" t="s">
+      <c r="Q101" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R99" s="5" t="s">
+      <c r="R101" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="2:5">
-      <c r="B100" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E100" s="9" t="s">
+    <row r="102" spans="2:5">
+      <c r="B102" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="101" spans="2:2">
-      <c r="B101" s="7" t="s">
+      <c r="C102" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="102" spans="2:2">
-      <c r="B102" s="7" t="s">
+      <c r="D102" s="9" t="s">
         <v>82</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3143,8 +3196,7 @@
     <mergeCell ref="B3:R3"/>
     <mergeCell ref="C5:R10"/>
     <mergeCell ref="C11:R16"/>
-    <mergeCell ref="C17:R19"/>
-    <mergeCell ref="C20:R20"/>
+    <mergeCell ref="C17:R20"/>
     <mergeCell ref="C21:R36"/>
     <mergeCell ref="B71:R71"/>
     <mergeCell ref="C73:R73"/>
@@ -3161,13 +3213,14 @@
     <mergeCell ref="C85:R85"/>
     <mergeCell ref="C86:R86"/>
     <mergeCell ref="B88:R88"/>
-    <mergeCell ref="B93:R93"/>
-    <mergeCell ref="B98:R98"/>
+    <mergeCell ref="C92:R93"/>
+    <mergeCell ref="B95:R95"/>
+    <mergeCell ref="B100:R100"/>
   </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1641886364" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643161361" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3176,14 +3229,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641886364" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643161361" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3209,7 +3262,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -3304,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -3657,10 +3710,10 @@
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -3680,7 +3733,7 @@
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -3701,7 +3754,7 @@
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -3722,7 +3775,7 @@
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="21" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -3743,7 +3796,7 @@
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -3764,7 +3817,7 @@
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -3785,7 +3838,7 @@
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -3957,7 +4010,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1641886364" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643161361" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3966,14 +4019,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1641886364" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641886364" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643161361" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
devanagari glyph improvements and new encoding scheme wip
</commit_message>
<xml_diff>
--- a/PUA_allocation_chart.xlsx
+++ b/PUA_allocation_chart.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="torvald"/>
+  <fileSharing readOnlyRecommended="0" userName="installed"/>
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="28800" windowHeight="14130" tabRatio="500"/>
@@ -14,17 +14,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1643161361" val="1040" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1643161361" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1643161361" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1643161361"/>
+      <pm:revision xmlns:pm="smNativeData" day="1643533432" val="1040" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1643533432" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1643533432" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1643533432"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
   <si>
     <t>PUA Allocation Chart U+Fxxxx</t>
   </si>
@@ -107,12 +107,24 @@
     <t>F00F</t>
   </si>
   <si>
-    <t>Unassigned</t>
-  </si>
-  <si>
     <t>Devanagari Presentation Forms</t>
   </si>
   <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Consonants</t>
+  </si>
+  <si>
+    <t>ConsonantsHalf</t>
+  </si>
+  <si>
+    <t>ConsonantR</t>
+  </si>
+  <si>
+    <t>ConsonantRHalf</t>
+  </si>
+  <si>
     <t>Small ASCII Characters for Super/Subscript Composition Used Internally</t>
   </si>
   <si>
@@ -269,7 +281,7 @@
     <t>FFFC</t>
   </si>
   <si>
-    <t>Nul</t>
+    <t>Default</t>
   </si>
   <si>
     <t>BG</t>
@@ -332,7 +344,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _£_-;\-* #,##0.00\ _£_-;_-* &quot;-&quot;??\ _£_-;_-@_-"/>
     <numFmt numFmtId="1" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -340,7 +352,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -355,7 +367,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -371,7 +383,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="300" lang="default" weight="bold"/>
@@ -387,7 +399,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -403,7 +415,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -418,7 +430,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -434,10 +446,25 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643161361" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="9"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="180" lang="default"/>
+            <pm:cs face="Basic Roman" sz="180" lang="default"/>
+            <pm:ea face="Basic Roman" sz="180" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -462,7 +489,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -473,7 +500,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -484,7 +511,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -495,7 +522,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -506,7 +533,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -520,7 +547,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -531,7 +558,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643161361" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -553,7 +580,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
+          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
         </ext>
       </extLst>
     </border>
@@ -572,7 +599,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361">
+          <pm:border xmlns:pm="smNativeData" id="1643533432">
             <pm:line position="bottom" type="1" style="0" width="50" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
         </ext>
@@ -593,7 +620,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361">
+          <pm:border xmlns:pm="smNativeData" id="1643533432">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -614,7 +641,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361">
+          <pm:border xmlns:pm="smNativeData" id="1643533432">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -638,7 +665,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
+          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
         </ext>
       </extLst>
     </border>
@@ -657,7 +684,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361">
+          <pm:border xmlns:pm="smNativeData" id="1643533432">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -680,7 +707,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361">
+          <pm:border xmlns:pm="smNativeData" id="1643533432">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
           </pm:border>
@@ -702,7 +729,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361">
+          <pm:border xmlns:pm="smNativeData" id="1643533432">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -725,7 +752,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361">
+          <pm:border xmlns:pm="smNativeData" id="1643533432">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -746,7 +773,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
+          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
         </ext>
       </extLst>
     </border>
@@ -765,7 +792,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643161361"/>
+          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
         </ext>
       </extLst>
     </border>
@@ -777,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
@@ -837,6 +864,9 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -848,10 +878,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1643161361" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1643533432" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1643161361" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1643533432" count="6">
         <pm:color name="Color 24" rgb="44546A"/>
         <pm:color name="Color 25" rgb="FFFFCC"/>
         <pm:color name="Color 26" rgb="A5A5A5"/>
@@ -1120,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T105"/>
+  <dimension ref="A1:U137"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -1552,9 +1582,7 @@
       <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -1571,13 +1599,13 @@
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
     </row>
-    <row r="21" spans="2:18">
+    <row r="21" spans="2:21">
       <c r="B21" s="7" t="str">
         <f>"F01"&amp;RIGHT(B5,1)</f>
         <v>F010</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -1594,8 +1622,11 @@
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
-    </row>
-    <row r="22" spans="2:18">
+      <c r="U21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21">
       <c r="B22" s="7" t="str">
         <f>"F01"&amp;RIGHT(B6,1)</f>
         <v>F011</v>
@@ -1616,8 +1647,11 @@
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
-    </row>
-    <row r="23" spans="2:18">
+      <c r="U22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21">
       <c r="B23" s="7" t="str">
         <f>"F01"&amp;RIGHT(B7,1)</f>
         <v>F012</v>
@@ -1638,8 +1672,11 @@
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
-    </row>
-    <row r="24" spans="2:18">
+      <c r="U23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21">
       <c r="B24" s="7" t="str">
         <f>"F01"&amp;RIGHT(B8,1)</f>
         <v>F013</v>
@@ -1660,8 +1697,11 @@
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
-    </row>
-    <row r="25" spans="2:18">
+      <c r="U24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21">
       <c r="B25" s="7" t="str">
         <f>"F01"&amp;RIGHT(B9,1)</f>
         <v>F014</v>
@@ -1682,8 +1722,11 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
-    </row>
-    <row r="26" spans="2:18">
+      <c r="U25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21">
       <c r="B26" s="7" t="str">
         <f>"F01"&amp;RIGHT(B10,1)</f>
         <v>F015</v>
@@ -1704,8 +1747,11 @@
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
-    </row>
-    <row r="27" spans="2:18">
+      <c r="U26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21">
       <c r="B27" s="7" t="str">
         <f>"F01"&amp;RIGHT(B11,1)</f>
         <v>F016</v>
@@ -1726,8 +1772,11 @@
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
-    </row>
-    <row r="28" spans="2:18">
+      <c r="U27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21">
       <c r="B28" s="7" t="str">
         <f>"F01"&amp;RIGHT(B12,1)</f>
         <v>F017</v>
@@ -1748,8 +1797,11 @@
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
-    </row>
-    <row r="29" spans="2:18">
+      <c r="U28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21">
       <c r="B29" s="7" t="str">
         <f>"F01"&amp;RIGHT(B13,1)</f>
         <v>F018</v>
@@ -1770,8 +1822,11 @@
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
-    </row>
-    <row r="30" spans="2:18">
+      <c r="U29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21">
       <c r="B30" s="7" t="str">
         <f>"F01"&amp;RIGHT(B14,1)</f>
         <v>F019</v>
@@ -1792,8 +1847,11 @@
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
-    </row>
-    <row r="31" spans="2:18">
+      <c r="U30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21">
       <c r="B31" s="7" t="str">
         <f>"F01"&amp;RIGHT(B15,1)</f>
         <v>F01A</v>
@@ -1814,8 +1872,11 @@
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
-    </row>
-    <row r="32" spans="2:18">
+      <c r="U31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21">
       <c r="B32" s="7" t="str">
         <f>"F01"&amp;RIGHT(B16,1)</f>
         <v>F01B</v>
@@ -1836,8 +1897,11 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
-    </row>
-    <row r="33" spans="2:18">
+      <c r="U32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21">
       <c r="B33" s="7" t="str">
         <f>"F01"&amp;RIGHT(B17,1)</f>
         <v>F01C</v>
@@ -1858,8 +1922,11 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
-    </row>
-    <row r="34" spans="2:18">
+      <c r="U33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21">
       <c r="B34" s="7" t="str">
         <f>"F01"&amp;RIGHT(B18,1)</f>
         <v>F01D</v>
@@ -1880,8 +1947,11 @@
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
-    </row>
-    <row r="35" spans="2:18">
+      <c r="U34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21">
       <c r="B35" s="7" t="str">
         <f>"F01"&amp;RIGHT(B19,1)</f>
         <v>F01E</v>
@@ -1902,8 +1972,11 @@
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
-    </row>
-    <row r="36" spans="2:18">
+      <c r="U35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21">
       <c r="B36" s="7" t="str">
         <f>"F01"&amp;RIGHT(B20,1)</f>
         <v>F01F</v>
@@ -1924,8 +1997,11 @@
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
       <c r="R36" s="15"/>
-    </row>
-    <row r="37" spans="2:18">
+      <c r="U36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21">
       <c r="B37" s="7" t="str">
         <f>"F02"&amp;RIGHT(B21,1)</f>
         <v>F020</v>
@@ -1946,8 +2022,11 @@
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
-    </row>
-    <row r="38" spans="2:18">
+      <c r="U37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21">
       <c r="B38" s="7" t="str">
         <f>"F02"&amp;RIGHT(B22,1)</f>
         <v>F021</v>
@@ -1968,8 +2047,11 @@
       <c r="P38" s="15"/>
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
-    </row>
-    <row r="39" spans="2:18">
+      <c r="U38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21">
       <c r="B39" s="7" t="str">
         <f>"F02"&amp;RIGHT(B23,1)</f>
         <v>F022</v>
@@ -1990,8 +2072,11 @@
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
-    </row>
-    <row r="40" spans="2:18">
+      <c r="U39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21">
       <c r="B40" s="7" t="str">
         <f>"F02"&amp;RIGHT(B24,1)</f>
         <v>F023</v>
@@ -2012,8 +2097,11 @@
       <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
-    </row>
-    <row r="41" spans="2:18">
+      <c r="U40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21">
       <c r="B41" s="7" t="str">
         <f>"F02"&amp;RIGHT(B25,1)</f>
         <v>F024</v>
@@ -2034,8 +2122,11 @@
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
-    </row>
-    <row r="42" spans="2:18">
+      <c r="U41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21">
       <c r="B42" s="7" t="str">
         <f>"F02"&amp;RIGHT(B26,1)</f>
         <v>F025</v>
@@ -2056,8 +2147,11 @@
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
-    </row>
-    <row r="43" spans="2:18">
+      <c r="U42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21">
       <c r="B43" s="7" t="str">
         <f>"F02"&amp;RIGHT(B27,1)</f>
         <v>F026</v>
@@ -2078,8 +2172,11 @@
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
-    </row>
-    <row r="44" spans="2:18">
+      <c r="U43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21">
       <c r="B44" s="7" t="str">
         <f>"F02"&amp;RIGHT(B28,1)</f>
         <v>F027</v>
@@ -2100,8 +2197,11 @@
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
-    </row>
-    <row r="45" spans="2:18">
+      <c r="U44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21">
       <c r="B45" s="7" t="str">
         <f>"F02"&amp;RIGHT(B29,1)</f>
         <v>F028</v>
@@ -2122,8 +2222,11 @@
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
-    </row>
-    <row r="46" spans="2:18">
+      <c r="U45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21">
       <c r="B46" s="7" t="str">
         <f>"F02"&amp;RIGHT(B30,1)</f>
         <v>F029</v>
@@ -2144,8 +2247,11 @@
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
-    </row>
-    <row r="47" spans="2:18">
+      <c r="U46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21">
       <c r="B47" s="7" t="str">
         <f>"F02"&amp;RIGHT(B31,1)</f>
         <v>F02A</v>
@@ -2166,8 +2272,11 @@
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
-    </row>
-    <row r="48" spans="2:18">
+      <c r="U47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21">
       <c r="B48" s="7" t="str">
         <f>"F02"&amp;RIGHT(B32,1)</f>
         <v>F02B</v>
@@ -2188,8 +2297,11 @@
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
-    </row>
-    <row r="49" spans="2:18">
+      <c r="U48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21">
       <c r="B49" s="7" t="str">
         <f>"F02"&amp;RIGHT(B33,1)</f>
         <v>F02C</v>
@@ -2210,8 +2322,11 @@
       <c r="P49" s="15"/>
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
-    </row>
-    <row r="50" spans="2:18">
+      <c r="U49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21">
       <c r="B50" s="7" t="str">
         <f>"F02"&amp;RIGHT(B34,1)</f>
         <v>F02D</v>
@@ -2232,8 +2347,11 @@
       <c r="P50" s="15"/>
       <c r="Q50" s="15"/>
       <c r="R50" s="15"/>
-    </row>
-    <row r="51" spans="2:18">
+      <c r="U50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21">
       <c r="B51" s="7" t="str">
         <f>"F02"&amp;RIGHT(B35,1)</f>
         <v>F02E</v>
@@ -2254,8 +2372,11 @@
       <c r="P51" s="15"/>
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
-    </row>
-    <row r="52" spans="2:18">
+      <c r="U51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21">
       <c r="B52" s="7" t="str">
         <f>"F02"&amp;RIGHT(B36,1)</f>
         <v>F02F</v>
@@ -2276,11 +2397,14 @@
       <c r="P52" s="15"/>
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
-    </row>
-    <row r="53" spans="2:18">
+      <c r="U52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21">
       <c r="B53" s="7" t="str">
-        <f>"F02"&amp;RIGHT(B37,1)</f>
-        <v>F020</v>
+        <f>"F03"&amp;RIGHT(B37,1)</f>
+        <v>F030</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
@@ -2298,8 +2422,11 @@
       <c r="P53" s="15"/>
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
-    </row>
-    <row r="54" spans="2:18">
+      <c r="U53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21">
       <c r="B54" s="7" t="str">
         <f>"F03"&amp;RIGHT(B38,1)</f>
         <v>F031</v>
@@ -2320,8 +2447,11 @@
       <c r="P54" s="15"/>
       <c r="Q54" s="15"/>
       <c r="R54" s="15"/>
-    </row>
-    <row r="55" spans="2:18">
+      <c r="U54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21">
       <c r="B55" s="7" t="str">
         <f>"F03"&amp;RIGHT(B39,1)</f>
         <v>F032</v>
@@ -2342,8 +2472,11 @@
       <c r="P55" s="15"/>
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
-    </row>
-    <row r="56" spans="2:18">
+      <c r="U55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21">
       <c r="B56" s="7" t="str">
         <f>"F03"&amp;RIGHT(B40,1)</f>
         <v>F033</v>
@@ -2364,8 +2497,11 @@
       <c r="P56" s="15"/>
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
-    </row>
-    <row r="57" spans="2:18">
+      <c r="U56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21">
       <c r="B57" s="7" t="str">
         <f>"F03"&amp;RIGHT(B41,1)</f>
         <v>F034</v>
@@ -2386,8 +2522,11 @@
       <c r="P57" s="15"/>
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
-    </row>
-    <row r="58" spans="2:18">
+      <c r="U57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:21">
       <c r="B58" s="7" t="str">
         <f>"F03"&amp;RIGHT(B42,1)</f>
         <v>F035</v>
@@ -2408,8 +2547,11 @@
       <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
-    </row>
-    <row r="59" spans="2:18">
+      <c r="U58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21">
       <c r="B59" s="7" t="str">
         <f>"F03"&amp;RIGHT(B43,1)</f>
         <v>F036</v>
@@ -2430,8 +2572,11 @@
       <c r="P59" s="15"/>
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
-    </row>
-    <row r="60" spans="2:18">
+      <c r="U59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21">
       <c r="B60" s="7" t="str">
         <f>"F03"&amp;RIGHT(B44,1)</f>
         <v>F037</v>
@@ -2452,8 +2597,11 @@
       <c r="P60" s="15"/>
       <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
-    </row>
-    <row r="61" spans="2:18">
+      <c r="U60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21">
       <c r="B61" s="7" t="str">
         <f>"F03"&amp;RIGHT(B45,1)</f>
         <v>F038</v>
@@ -2474,8 +2622,11 @@
       <c r="P61" s="15"/>
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
-    </row>
-    <row r="62" spans="2:18">
+      <c r="U61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21">
       <c r="B62" s="7" t="str">
         <f>"F03"&amp;RIGHT(B46,1)</f>
         <v>F039</v>
@@ -2496,8 +2647,11 @@
       <c r="P62" s="15"/>
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
-    </row>
-    <row r="63" spans="2:18">
+      <c r="U62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21">
       <c r="B63" s="7" t="str">
         <f>"F03"&amp;RIGHT(B47,1)</f>
         <v>F03A</v>
@@ -2518,8 +2672,11 @@
       <c r="P63" s="15"/>
       <c r="Q63" s="15"/>
       <c r="R63" s="15"/>
-    </row>
-    <row r="64" spans="2:18">
+      <c r="U63" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21">
       <c r="B64" s="7" t="str">
         <f>"F03"&amp;RIGHT(B48,1)</f>
         <v>F03B</v>
@@ -2540,8 +2697,11 @@
       <c r="P64" s="15"/>
       <c r="Q64" s="15"/>
       <c r="R64" s="15"/>
-    </row>
-    <row r="65" spans="2:18">
+      <c r="U64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="2:21">
       <c r="B65" s="7" t="str">
         <f>"F03"&amp;RIGHT(B49,1)</f>
         <v>F03C</v>
@@ -2562,8 +2722,11 @@
       <c r="P65" s="15"/>
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
-    </row>
-    <row r="66" spans="2:18">
+      <c r="U65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="2:21">
       <c r="B66" s="7" t="str">
         <f>"F03"&amp;RIGHT(B50,1)</f>
         <v>F03D</v>
@@ -2584,8 +2747,11 @@
       <c r="P66" s="15"/>
       <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
-    </row>
-    <row r="67" spans="2:18">
+      <c r="U66" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="2:21">
       <c r="B67" s="7" t="str">
         <f>"F03"&amp;RIGHT(B51,1)</f>
         <v>F03E</v>
@@ -2606,8 +2772,11 @@
       <c r="P67" s="15"/>
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
-    </row>
-    <row r="68" spans="2:18">
+      <c r="U67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="2:21">
       <c r="B68" s="7" t="str">
         <f>"F03"&amp;RIGHT(B52,1)</f>
         <v>F03F</v>
@@ -2628,8 +2797,15 @@
       <c r="P68" s="15"/>
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
-    </row>
-    <row r="69" spans="3:18">
+      <c r="U68" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="2:21">
+      <c r="B69" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B53,1)</f>
+        <v>F040</v>
+      </c>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
@@ -2646,309 +2822,521 @@
       <c r="P69" s="15"/>
       <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
-    </row>
-    <row r="71" spans="2:19">
-      <c r="B71" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
-      <c r="J71" s="17"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="17"/>
-      <c r="R71" s="17"/>
-      <c r="S71" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="2:18">
-      <c r="B72" s="8"/>
-      <c r="C72" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E72" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F72" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G72" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H72" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I72" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J72" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="K72" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="L72" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="M72" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N72" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O72" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P72" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q72" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R72" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="2:19">
-      <c r="B73" s="7" t="s">
+      <c r="U69" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="9" t="s">
+    </row>
+    <row r="70" spans="2:21">
+      <c r="B70" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B54,1)</f>
+        <v>F041</v>
+      </c>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="U70" t="s">
         <v>32</v>
       </c>
-      <c r="S73" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3">
-      <c r="B74" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3">
-      <c r="B75" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3">
-      <c r="B76" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3">
-      <c r="B77" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3">
-      <c r="B78" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="80" spans="2:18">
-      <c r="B80" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
-      <c r="P80" s="17"/>
-      <c r="Q80" s="17"/>
-      <c r="R80" s="17"/>
-    </row>
-    <row r="81" spans="2:3">
-      <c r="B81" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3">
-      <c r="B82" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3">
-      <c r="B83" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3">
-      <c r="B84" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3">
-      <c r="B85" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3">
-      <c r="B86" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>56</v>
-      </c>
+    </row>
+    <row r="71" spans="2:21">
+      <c r="B71" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B55,1)</f>
+        <v>F042</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="U71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="2:21">
+      <c r="B72" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B56,1)</f>
+        <v>F043</v>
+      </c>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="U72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21">
+      <c r="B73" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B57,1)</f>
+        <v>F044</v>
+      </c>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="U73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="2:21">
+      <c r="B74" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B58,1)</f>
+        <v>F045</v>
+      </c>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="U74" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="2:21">
+      <c r="B75" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B59,1)</f>
+        <v>F046</v>
+      </c>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="U75" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="2:21">
+      <c r="B76" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B60,1)</f>
+        <v>F047</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="U76" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="2:21">
+      <c r="B77" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B61,1)</f>
+        <v>F048</v>
+      </c>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="U77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21">
+      <c r="B78" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B62,1)</f>
+        <v>F049</v>
+      </c>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="U78" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="2:21">
+      <c r="B79" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B63,1)</f>
+        <v>F04A</v>
+      </c>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15"/>
+      <c r="U79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="2:21">
+      <c r="B80" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B64,1)</f>
+        <v>F04B</v>
+      </c>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15"/>
+      <c r="U80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="2:21">
+      <c r="B81" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B65,1)</f>
+        <v>F04C</v>
+      </c>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15"/>
+      <c r="Q81" s="15"/>
+      <c r="R81" s="15"/>
+      <c r="U81" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="2:21">
+      <c r="B82" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B66,1)</f>
+        <v>F04D</v>
+      </c>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="15"/>
+      <c r="Q82" s="15"/>
+      <c r="R82" s="15"/>
+      <c r="U82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="2:21">
+      <c r="B83" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B67,1)</f>
+        <v>F04E</v>
+      </c>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
+      <c r="P83" s="15"/>
+      <c r="Q83" s="15"/>
+      <c r="R83" s="15"/>
+      <c r="U83" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="2:21">
+      <c r="B84" s="7" t="str">
+        <f>"F04"&amp;RIGHT(B68,1)</f>
+        <v>F04F</v>
+      </c>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="15"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="O84" s="15"/>
+      <c r="P84" s="15"/>
+      <c r="Q84" s="15"/>
+      <c r="R84" s="15"/>
+      <c r="U84" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18">
+      <c r="B85"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+    </row>
+    <row r="86" spans="2:18">
+      <c r="B86"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+    </row>
+    <row r="87" spans="2:18">
+      <c r="B87"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="15"/>
+      <c r="O87" s="15"/>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="15"/>
+      <c r="R87" s="15"/>
     </row>
     <row r="88" spans="2:18">
-      <c r="B88" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="12"/>
-      <c r="K88" s="12"/>
-      <c r="L88" s="12"/>
-      <c r="M88" s="12"/>
-      <c r="N88" s="12"/>
-      <c r="O88" s="12"/>
-      <c r="P88" s="12"/>
-      <c r="Q88" s="12"/>
-      <c r="R88" s="13"/>
+      <c r="B88"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="15"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15"/>
+      <c r="O88" s="15"/>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="15"/>
     </row>
     <row r="89" spans="2:18">
-      <c r="B89" s="8"/>
-      <c r="C89" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D89" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E89" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F89" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G89" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H89" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I89" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J89" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="K89" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="L89" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P89" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q89" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R89" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="2:20">
-      <c r="B90" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D90" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="S90" t="s">
-        <v>61</v>
-      </c>
-      <c r="T90" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="2:19">
-      <c r="B91" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="S91" t="s">
-        <v>65</v>
-      </c>
+      <c r="B89"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="15"/>
+      <c r="M89" s="15"/>
+      <c r="N89" s="15"/>
+      <c r="O89" s="15"/>
+      <c r="P89" s="15"/>
+      <c r="Q89" s="15"/>
+      <c r="R89" s="15"/>
+    </row>
+    <row r="90" spans="2:18">
+      <c r="B90"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="15"/>
+      <c r="L90" s="15"/>
+      <c r="M90" s="15"/>
+      <c r="N90" s="15"/>
+      <c r="O90" s="15"/>
+      <c r="P90" s="15"/>
+      <c r="Q90" s="15"/>
+      <c r="R90" s="15"/>
+    </row>
+    <row r="91" spans="2:18">
+      <c r="B91"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="15"/>
+      <c r="M91" s="15"/>
+      <c r="N91" s="15"/>
+      <c r="O91" s="15"/>
+      <c r="P91" s="15"/>
+      <c r="Q91" s="15"/>
+      <c r="R91" s="15"/>
     </row>
     <row r="92" spans="2:18">
-      <c r="B92" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>67</v>
-      </c>
+      <c r="B92"/>
+      <c r="C92" s="15"/>
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
       <c r="F92" s="15"/>
@@ -2966,9 +3354,7 @@
       <c r="R92" s="15"/>
     </row>
     <row r="93" spans="2:18">
-      <c r="B93" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="B93"/>
       <c r="C93" s="15"/>
       <c r="D93" s="15"/>
       <c r="E93" s="15"/>
@@ -2986,208 +3372,698 @@
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
     </row>
+    <row r="94" spans="2:18">
+      <c r="B94"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="15"/>
+      <c r="M94" s="15"/>
+      <c r="N94" s="15"/>
+      <c r="O94" s="15"/>
+      <c r="P94" s="15"/>
+      <c r="Q94" s="15"/>
+      <c r="R94" s="15"/>
+    </row>
     <row r="95" spans="2:18">
-      <c r="B95" s="11" t="s">
+      <c r="B95"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="15"/>
+      <c r="N95" s="15"/>
+      <c r="O95" s="15"/>
+      <c r="P95" s="15"/>
+      <c r="Q95" s="15"/>
+      <c r="R95" s="15"/>
+    </row>
+    <row r="96" spans="2:18">
+      <c r="B96"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="15"/>
+      <c r="L96" s="15"/>
+      <c r="M96" s="15"/>
+      <c r="N96" s="15"/>
+      <c r="O96" s="15"/>
+      <c r="P96" s="15"/>
+      <c r="Q96" s="15"/>
+      <c r="R96" s="15"/>
+    </row>
+    <row r="97" spans="2:18">
+      <c r="B97"/>
+      <c r="C97" s="15"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="15"/>
+      <c r="M97" s="15"/>
+      <c r="N97" s="15"/>
+      <c r="O97" s="15"/>
+      <c r="P97" s="15"/>
+      <c r="Q97" s="15"/>
+      <c r="R97" s="15"/>
+    </row>
+    <row r="98" spans="2:18">
+      <c r="B98"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="15"/>
+      <c r="O98" s="15"/>
+      <c r="P98" s="15"/>
+      <c r="Q98" s="15"/>
+      <c r="R98" s="15"/>
+    </row>
+    <row r="99" spans="2:18">
+      <c r="B99"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="15"/>
+      <c r="L99" s="15"/>
+      <c r="M99" s="15"/>
+      <c r="N99" s="15"/>
+      <c r="O99" s="15"/>
+      <c r="P99" s="15"/>
+      <c r="Q99" s="15"/>
+      <c r="R99" s="15"/>
+    </row>
+    <row r="100" spans="2:18">
+      <c r="B100"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="15"/>
+      <c r="K100" s="15"/>
+      <c r="L100" s="15"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="15"/>
+      <c r="O100" s="15"/>
+      <c r="P100" s="15"/>
+      <c r="Q100" s="15"/>
+      <c r="R100" s="15"/>
+    </row>
+    <row r="101" spans="3:18">
+      <c r="C101" s="15"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15"/>
+      <c r="J101" s="15"/>
+      <c r="K101" s="15"/>
+      <c r="L101" s="15"/>
+      <c r="M101" s="15"/>
+      <c r="N101" s="15"/>
+      <c r="O101" s="15"/>
+      <c r="P101" s="15"/>
+      <c r="Q101" s="15"/>
+      <c r="R101" s="15"/>
+    </row>
+    <row r="103" spans="2:19">
+      <c r="B103" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="17"/>
+      <c r="L103" s="17"/>
+      <c r="M103" s="17"/>
+      <c r="N103" s="17"/>
+      <c r="O103" s="17"/>
+      <c r="P103" s="17"/>
+      <c r="Q103" s="17"/>
+      <c r="R103" s="17"/>
+      <c r="S103" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="104" spans="2:18">
+      <c r="B104" s="8"/>
+      <c r="C104" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D104" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F104" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G104" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H104" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I104" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="J104" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K104" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="L104" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N104" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O104" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P104" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q104" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R104" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="2:19">
+      <c r="B105" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S105" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3">
+      <c r="B106" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3">
+      <c r="B107" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3">
+      <c r="B108" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3">
+      <c r="B109" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3">
+      <c r="B110" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="112" spans="2:18">
+      <c r="B112" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="17"/>
+      <c r="H112" s="17"/>
+      <c r="I112" s="17"/>
+      <c r="J112" s="17"/>
+      <c r="K112" s="17"/>
+      <c r="L112" s="17"/>
+      <c r="M112" s="17"/>
+      <c r="N112" s="17"/>
+      <c r="O112" s="17"/>
+      <c r="P112" s="17"/>
+      <c r="Q112" s="17"/>
+      <c r="R112" s="17"/>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="B113" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3">
+      <c r="B114" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
+      <c r="B115" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3">
+      <c r="B116" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3">
+      <c r="B117" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3">
+      <c r="B118" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="2:18">
+      <c r="B120" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="12"/>
+      <c r="I120" s="12"/>
+      <c r="J120" s="12"/>
+      <c r="K120" s="12"/>
+      <c r="L120" s="12"/>
+      <c r="M120" s="12"/>
+      <c r="N120" s="12"/>
+      <c r="O120" s="12"/>
+      <c r="P120" s="12"/>
+      <c r="Q120" s="12"/>
+      <c r="R120" s="13"/>
+    </row>
+    <row r="121" spans="2:18">
+      <c r="B121" s="8"/>
+      <c r="C121" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E121" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F121" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G121" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H121" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I121" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="J121" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K121" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="L121" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M121" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N121" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O121" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P121" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q121" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R121" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="2:20">
+      <c r="B122" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="S122" t="s">
+        <v>65</v>
+      </c>
+      <c r="T122" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="123" spans="2:19">
+      <c r="B123" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S123" t="s">
         <v>69</v>
       </c>
-      <c r="C95" s="12"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="12"/>
-      <c r="I95" s="12"/>
-      <c r="J95" s="12"/>
-      <c r="K95" s="12"/>
-      <c r="L95" s="12"/>
-      <c r="M95" s="12"/>
-      <c r="N95" s="12"/>
-      <c r="O95" s="12"/>
-      <c r="P95" s="12"/>
-      <c r="Q95" s="12"/>
-      <c r="R95" s="13"/>
-    </row>
-    <row r="96" spans="2:18">
-      <c r="B96" s="8"/>
-      <c r="C96" s="5" t="n">
+    </row>
+    <row r="124" spans="2:18">
+      <c r="B124" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D124" s="15"/>
+      <c r="E124" s="15"/>
+      <c r="F124" s="15"/>
+      <c r="G124" s="15"/>
+      <c r="H124" s="15"/>
+      <c r="I124" s="15"/>
+      <c r="J124" s="15"/>
+      <c r="K124" s="15"/>
+      <c r="L124" s="15"/>
+      <c r="M124" s="15"/>
+      <c r="N124" s="15"/>
+      <c r="O124" s="15"/>
+      <c r="P124" s="15"/>
+      <c r="Q124" s="15"/>
+      <c r="R124" s="15"/>
+    </row>
+    <row r="125" spans="2:18">
+      <c r="B125" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="15"/>
+      <c r="H125" s="15"/>
+      <c r="I125" s="15"/>
+      <c r="J125" s="15"/>
+      <c r="K125" s="15"/>
+      <c r="L125" s="15"/>
+      <c r="M125" s="15"/>
+      <c r="N125" s="15"/>
+      <c r="O125" s="15"/>
+      <c r="P125" s="15"/>
+      <c r="Q125" s="15"/>
+      <c r="R125" s="15"/>
+    </row>
+    <row r="127" spans="2:18">
+      <c r="B127" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
+      <c r="I127" s="12"/>
+      <c r="J127" s="12"/>
+      <c r="K127" s="12"/>
+      <c r="L127" s="12"/>
+      <c r="M127" s="12"/>
+      <c r="N127" s="12"/>
+      <c r="O127" s="12"/>
+      <c r="P127" s="12"/>
+      <c r="Q127" s="12"/>
+      <c r="R127" s="13"/>
+    </row>
+    <row r="128" spans="2:18">
+      <c r="B128" s="8"/>
+      <c r="C128" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D96" s="5" t="n">
+      <c r="D128" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E96" s="5" t="n">
+      <c r="E128" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F96" s="5" t="n">
+      <c r="F128" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G96" s="5" t="n">
+      <c r="G128" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H96" s="5" t="n">
+      <c r="H128" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I96" s="5" t="n">
+      <c r="I128" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J96" s="5" t="n">
+      <c r="J128" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K96" s="5" t="n">
+      <c r="K128" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L96" s="5" t="n">
+      <c r="L128" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M96" s="5" t="s">
+      <c r="M128" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N96" s="5" t="s">
+      <c r="N128" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O96" s="5" t="s">
+      <c r="O128" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P96" s="5" t="s">
+      <c r="P128" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q96" s="5" t="s">
+      <c r="Q128" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R96" s="5" t="s">
+      <c r="R128" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="2:19">
-      <c r="B97" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F97" s="9" t="s">
+    <row r="129" spans="2:19">
+      <c r="B129" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="S97" t="s">
+      <c r="C129" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="98" spans="2:19">
-      <c r="B98" s="7" t="s">
+      <c r="D129" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="R98" s="9" t="s">
+      <c r="E129" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="S98" t="s">
+      <c r="F129" s="9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="100" spans="2:18">
-      <c r="B100" s="11" t="s">
+      <c r="S129" t="s">
         <v>79</v>
       </c>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="12"/>
-      <c r="K100" s="12"/>
-      <c r="L100" s="12"/>
-      <c r="M100" s="12"/>
-      <c r="N100" s="12"/>
-      <c r="O100" s="12"/>
-      <c r="P100" s="12"/>
-      <c r="Q100" s="12"/>
-      <c r="R100" s="13"/>
-    </row>
-    <row r="101" spans="2:18">
-      <c r="B101" s="8"/>
-      <c r="C101" s="5" t="n">
+    </row>
+    <row r="130" spans="2:19">
+      <c r="B130" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="R130" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S130" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="2:18">
+      <c r="B132" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C132" s="12"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
+      <c r="G132" s="12"/>
+      <c r="H132" s="12"/>
+      <c r="I132" s="12"/>
+      <c r="J132" s="12"/>
+      <c r="K132" s="12"/>
+      <c r="L132" s="12"/>
+      <c r="M132" s="12"/>
+      <c r="N132" s="12"/>
+      <c r="O132" s="12"/>
+      <c r="P132" s="12"/>
+      <c r="Q132" s="12"/>
+      <c r="R132" s="13"/>
+    </row>
+    <row r="133" spans="2:18">
+      <c r="B133" s="8"/>
+      <c r="C133" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D101" s="5" t="n">
+      <c r="D133" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E101" s="5" t="n">
+      <c r="E133" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F101" s="5" t="n">
+      <c r="F133" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G101" s="5" t="n">
+      <c r="G133" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H101" s="5" t="n">
+      <c r="H133" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I101" s="5" t="n">
+      <c r="I133" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J101" s="5" t="n">
+      <c r="J133" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="K101" s="5" t="n">
+      <c r="K133" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="L101" s="5" t="n">
+      <c r="L133" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M101" s="5" t="s">
+      <c r="M133" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N101" s="5" t="s">
+      <c r="N133" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O101" s="5" t="s">
+      <c r="O133" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P101" s="5" t="s">
+      <c r="P133" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q101" s="5" t="s">
+      <c r="Q133" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R101" s="5" t="s">
+      <c r="R133" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="2:5">
-      <c r="B102" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2">
-      <c r="B103" s="7" t="s">
+    <row r="134" spans="2:5">
+      <c r="B134" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="104" spans="2:2">
-      <c r="B104" s="7" t="s">
+      <c r="C134" s="23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="105" spans="2:2">
-      <c r="B105" s="7" t="s">
+      <c r="D134" s="9" t="s">
         <v>86</v>
+      </c>
+      <c r="E134" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3197,30 +4073,30 @@
     <mergeCell ref="C5:R10"/>
     <mergeCell ref="C11:R16"/>
     <mergeCell ref="C17:R20"/>
-    <mergeCell ref="C21:R36"/>
-    <mergeCell ref="B71:R71"/>
-    <mergeCell ref="C73:R73"/>
-    <mergeCell ref="C74:R74"/>
-    <mergeCell ref="C75:R75"/>
-    <mergeCell ref="C76:R76"/>
-    <mergeCell ref="C77:R77"/>
-    <mergeCell ref="C78:R78"/>
-    <mergeCell ref="B80:R80"/>
-    <mergeCell ref="C81:R81"/>
-    <mergeCell ref="C82:R82"/>
-    <mergeCell ref="C83:R83"/>
-    <mergeCell ref="C84:R84"/>
-    <mergeCell ref="C85:R85"/>
-    <mergeCell ref="C86:R86"/>
-    <mergeCell ref="B88:R88"/>
-    <mergeCell ref="C92:R93"/>
-    <mergeCell ref="B95:R95"/>
-    <mergeCell ref="B100:R100"/>
+    <mergeCell ref="C21:R84"/>
+    <mergeCell ref="B103:R103"/>
+    <mergeCell ref="C105:R105"/>
+    <mergeCell ref="C106:R106"/>
+    <mergeCell ref="C107:R107"/>
+    <mergeCell ref="C108:R108"/>
+    <mergeCell ref="C109:R109"/>
+    <mergeCell ref="C110:R110"/>
+    <mergeCell ref="B112:R112"/>
+    <mergeCell ref="C113:R113"/>
+    <mergeCell ref="C114:R114"/>
+    <mergeCell ref="C115:R115"/>
+    <mergeCell ref="C116:R116"/>
+    <mergeCell ref="C117:R117"/>
+    <mergeCell ref="C118:R118"/>
+    <mergeCell ref="B120:R120"/>
+    <mergeCell ref="C124:R125"/>
+    <mergeCell ref="B127:R127"/>
+    <mergeCell ref="B132:R132"/>
   </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643161361" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643533432" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3229,14 +4105,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643161361" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643533432" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3262,7 +4138,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="16" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -3357,7 +4233,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -3710,10 +4586,10 @@
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -3733,7 +4609,7 @@
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="7" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -3754,7 +4630,7 @@
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -3775,7 +4651,7 @@
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="21" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -3796,7 +4672,7 @@
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="7" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -3817,7 +4693,7 @@
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="7" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -3838,7 +4714,7 @@
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -4010,7 +4886,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643161361" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643533432" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4019,14 +4895,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643161361" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643161361" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643533432" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
fixed a bug where diacritics with align right would not get positioned correctly
</commit_message>
<xml_diff>
--- a/PUA_allocation_chart.xlsx
+++ b/PUA_allocation_chart.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="installed"/>
+  <fileSharing readOnlyRecommended="0" userName="torvald"/>
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="28800" windowHeight="14130" tabRatio="500"/>
@@ -14,17 +14,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1643533432" val="1040" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1643533432" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1643533432" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1643533432"/>
+      <pm:revision xmlns:pm="smNativeData" day="1647928895" val="1042" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1647928895" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1647928895" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1647928895"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
   <si>
     <t>PUA Allocation Chart U+Fxxxx</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>ConsonantRHalf</t>
+  </si>
+  <si>
+    <t>Sundanese Presentation Forms</t>
   </si>
   <si>
     <t>Small ASCII Characters for Super/Subscript Composition Used Internally</t>
@@ -352,7 +355,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -367,7 +370,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -383,7 +386,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="300" lang="default" weight="bold"/>
@@ -399,7 +402,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -415,7 +418,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -430,7 +433,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -446,7 +449,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -461,7 +464,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643533432" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1647928895" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="180" lang="default"/>
             <pm:cs face="Basic Roman" sz="180" lang="default"/>
             <pm:ea face="Basic Roman" sz="180" lang="default"/>
@@ -489,7 +492,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1647928895" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -500,7 +503,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1647928895" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -511,7 +514,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1647928895" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -522,7 +525,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1647928895" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -533,7 +536,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1647928895" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -547,7 +550,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1647928895" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -558,7 +561,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643533432" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1647928895" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -580,7 +583,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
+          <pm:border xmlns:pm="smNativeData" id="1647928895"/>
         </ext>
       </extLst>
     </border>
@@ -599,7 +602,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432">
+          <pm:border xmlns:pm="smNativeData" id="1647928895">
             <pm:line position="bottom" type="1" style="0" width="50" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
         </ext>
@@ -620,7 +623,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432">
+          <pm:border xmlns:pm="smNativeData" id="1647928895">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -641,7 +644,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432">
+          <pm:border xmlns:pm="smNativeData" id="1647928895">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -665,7 +668,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
+          <pm:border xmlns:pm="smNativeData" id="1647928895"/>
         </ext>
       </extLst>
     </border>
@@ -684,7 +687,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432">
+          <pm:border xmlns:pm="smNativeData" id="1647928895">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -707,7 +710,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432">
+          <pm:border xmlns:pm="smNativeData" id="1647928895">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
           </pm:border>
@@ -729,7 +732,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432">
+          <pm:border xmlns:pm="smNativeData" id="1647928895">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -752,7 +755,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432">
+          <pm:border xmlns:pm="smNativeData" id="1647928895">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="9BC2E6"/>
           </pm:border>
         </ext>
@@ -773,7 +776,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
+          <pm:border xmlns:pm="smNativeData" id="1647928895"/>
         </ext>
       </extLst>
     </border>
@@ -792,7 +795,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643533432"/>
+          <pm:border xmlns:pm="smNativeData" id="1647928895"/>
         </ext>
       </extLst>
     </border>
@@ -837,7 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -852,7 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -878,10 +881,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1643533432" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1647928895" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1643533432" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1647928895" count="6">
         <pm:color name="Color 24" rgb="44546A"/>
         <pm:color name="Color 25" rgb="FFFFCC"/>
         <pm:color name="Color 26" rgb="A5A5A5"/>
@@ -1153,7 +1156,7 @@
   <dimension ref="A1:U137"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -3202,8 +3205,13 @@
       </c>
     </row>
     <row r="85" spans="2:18">
-      <c r="B85"/>
-      <c r="C85" s="15"/>
+      <c r="B85" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B69,1)</f>
+        <v>F050</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="D85" s="15"/>
       <c r="E85" s="15"/>
       <c r="F85" s="15"/>
@@ -3221,7 +3229,10 @@
       <c r="R85" s="15"/>
     </row>
     <row r="86" spans="2:18">
-      <c r="B86"/>
+      <c r="B86" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B70,1)</f>
+        <v>F051</v>
+      </c>
       <c r="C86" s="15"/>
       <c r="D86" s="15"/>
       <c r="E86" s="15"/>
@@ -3240,7 +3251,10 @@
       <c r="R86" s="15"/>
     </row>
     <row r="87" spans="2:18">
-      <c r="B87"/>
+      <c r="B87" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B71,1)</f>
+        <v>F052</v>
+      </c>
       <c r="C87" s="15"/>
       <c r="D87" s="15"/>
       <c r="E87" s="15"/>
@@ -3259,7 +3273,10 @@
       <c r="R87" s="15"/>
     </row>
     <row r="88" spans="2:18">
-      <c r="B88"/>
+      <c r="B88" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B72,1)</f>
+        <v>F053</v>
+      </c>
       <c r="C88" s="15"/>
       <c r="D88" s="15"/>
       <c r="E88" s="15"/>
@@ -3278,7 +3295,10 @@
       <c r="R88" s="15"/>
     </row>
     <row r="89" spans="2:18">
-      <c r="B89"/>
+      <c r="B89" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B73,1)</f>
+        <v>F054</v>
+      </c>
       <c r="C89" s="15"/>
       <c r="D89" s="15"/>
       <c r="E89" s="15"/>
@@ -3297,7 +3317,10 @@
       <c r="R89" s="15"/>
     </row>
     <row r="90" spans="2:18">
-      <c r="B90"/>
+      <c r="B90" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B74,1)</f>
+        <v>F055</v>
+      </c>
       <c r="C90" s="15"/>
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
@@ -3316,7 +3339,10 @@
       <c r="R90" s="15"/>
     </row>
     <row r="91" spans="2:18">
-      <c r="B91"/>
+      <c r="B91" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B75,1)</f>
+        <v>F056</v>
+      </c>
       <c r="C91" s="15"/>
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
@@ -3335,7 +3361,10 @@
       <c r="R91" s="15"/>
     </row>
     <row r="92" spans="2:18">
-      <c r="B92"/>
+      <c r="B92" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B76,1)</f>
+        <v>F057</v>
+      </c>
       <c r="C92" s="15"/>
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
@@ -3354,7 +3383,10 @@
       <c r="R92" s="15"/>
     </row>
     <row r="93" spans="2:18">
-      <c r="B93"/>
+      <c r="B93" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B77,1)</f>
+        <v>F058</v>
+      </c>
       <c r="C93" s="15"/>
       <c r="D93" s="15"/>
       <c r="E93" s="15"/>
@@ -3373,7 +3405,10 @@
       <c r="R93" s="15"/>
     </row>
     <row r="94" spans="2:18">
-      <c r="B94"/>
+      <c r="B94" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B78,1)</f>
+        <v>F059</v>
+      </c>
       <c r="C94" s="15"/>
       <c r="D94" s="15"/>
       <c r="E94" s="15"/>
@@ -3392,7 +3427,10 @@
       <c r="R94" s="15"/>
     </row>
     <row r="95" spans="2:18">
-      <c r="B95"/>
+      <c r="B95" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B79,1)</f>
+        <v>F05A</v>
+      </c>
       <c r="C95" s="15"/>
       <c r="D95" s="15"/>
       <c r="E95" s="15"/>
@@ -3411,7 +3449,10 @@
       <c r="R95" s="15"/>
     </row>
     <row r="96" spans="2:18">
-      <c r="B96"/>
+      <c r="B96" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B80,1)</f>
+        <v>F05B</v>
+      </c>
       <c r="C96" s="15"/>
       <c r="D96" s="15"/>
       <c r="E96" s="15"/>
@@ -3430,7 +3471,10 @@
       <c r="R96" s="15"/>
     </row>
     <row r="97" spans="2:18">
-      <c r="B97"/>
+      <c r="B97" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B81,1)</f>
+        <v>F05C</v>
+      </c>
       <c r="C97" s="15"/>
       <c r="D97" s="15"/>
       <c r="E97" s="15"/>
@@ -3449,7 +3493,10 @@
       <c r="R97" s="15"/>
     </row>
     <row r="98" spans="2:18">
-      <c r="B98"/>
+      <c r="B98" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B82,1)</f>
+        <v>F05D</v>
+      </c>
       <c r="C98" s="15"/>
       <c r="D98" s="15"/>
       <c r="E98" s="15"/>
@@ -3468,7 +3515,10 @@
       <c r="R98" s="15"/>
     </row>
     <row r="99" spans="2:18">
-      <c r="B99"/>
+      <c r="B99" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B83,1)</f>
+        <v>F05E</v>
+      </c>
       <c r="C99" s="15"/>
       <c r="D99" s="15"/>
       <c r="E99" s="15"/>
@@ -3487,7 +3537,10 @@
       <c r="R99" s="15"/>
     </row>
     <row r="100" spans="2:18">
-      <c r="B100"/>
+      <c r="B100" s="7" t="str">
+        <f>"F05"&amp;RIGHT(B84,1)</f>
+        <v>F05F</v>
+      </c>
       <c r="C100" s="15"/>
       <c r="D100" s="15"/>
       <c r="E100" s="15"/>
@@ -3525,7 +3578,7 @@
     </row>
     <row r="103" spans="2:19">
       <c r="B103" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C103" s="17"/>
       <c r="D103" s="17"/>
@@ -3544,7 +3597,7 @@
       <c r="Q103" s="17"/>
       <c r="R103" s="17"/>
       <c r="S103" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="104" spans="2:18">
@@ -3600,58 +3653,58 @@
     </row>
     <row r="105" spans="2:19">
       <c r="B105" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S105" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="2:3">
       <c r="B106" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="2:3">
       <c r="B107" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="108" spans="2:3">
       <c r="B108" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="109" spans="2:3">
       <c r="B109" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="112" spans="2:18">
       <c r="B112" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C112" s="17"/>
       <c r="D112" s="17"/>
@@ -3672,55 +3725,55 @@
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="115" spans="2:3">
       <c r="B115" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="116" spans="2:3">
       <c r="B116" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="117" spans="2:3">
       <c r="B117" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="118" spans="2:3">
       <c r="B118" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="120" spans="2:18">
       <c r="B120" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C120" s="12"/>
       <c r="D120" s="12"/>
@@ -3792,38 +3845,38 @@
     </row>
     <row r="122" spans="2:20">
       <c r="B122" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S122" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T122" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="123" spans="2:19">
       <c r="B123" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S123" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="124" spans="2:18">
       <c r="B124" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="15"/>
@@ -3843,7 +3896,7 @@
     </row>
     <row r="125" spans="2:18">
       <c r="B125" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C125" s="15"/>
       <c r="D125" s="15"/>
@@ -3864,7 +3917,7 @@
     </row>
     <row r="127" spans="2:18">
       <c r="B127" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C127" s="12"/>
       <c r="D127" s="12"/>
@@ -3936,38 +3989,38 @@
     </row>
     <row r="129" spans="2:19">
       <c r="B129" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S129" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="130" spans="2:19">
       <c r="B130" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="R130" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="S130" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="132" spans="2:18">
       <c r="B132" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C132" s="12"/>
       <c r="D132" s="12"/>
@@ -4039,41 +4092,42 @@
     </row>
     <row r="134" spans="2:5">
       <c r="B134" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="B3:R3"/>
     <mergeCell ref="C5:R10"/>
     <mergeCell ref="C11:R16"/>
     <mergeCell ref="C17:R20"/>
     <mergeCell ref="C21:R84"/>
+    <mergeCell ref="C85:R85"/>
     <mergeCell ref="B103:R103"/>
     <mergeCell ref="C105:R105"/>
     <mergeCell ref="C106:R106"/>
@@ -4096,7 +4150,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643533432" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1647928895" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4105,14 +4159,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1647928895" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1647928895" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643533432" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1647928895" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4138,7 +4192,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4233,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -4586,10 +4640,10 @@
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -4609,7 +4663,7 @@
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -4630,7 +4684,7 @@
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -4651,7 +4705,7 @@
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -4672,7 +4726,7 @@
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -4693,7 +4747,7 @@
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -4714,7 +4768,7 @@
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -4886,7 +4940,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643533432" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1647928895" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4895,14 +4949,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643533432" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1647928895" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1647928895" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643533432" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1647928895" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>